<commit_message>
Fixed Kannada and Sanskrit spreadsheets
</commit_message>
<xml_diff>
--- a/acharyan_captions_kannada.xlsx
+++ b/acharyan_captions_kannada.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\CODING\POSTER\Sri_Parakala_Poster_Template_300DPI\Parampara_Poster\parampara_poster_template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFC343CF-1100-4226-9A98-3D5FC63078EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92CA9DD5-BFA8-49A9-B6CF-A879AB1904CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5110" yWindow="3240" windowWidth="28800" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="40110" yWindow="1100" windowWidth="27580" windowHeight="19070" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="acharyan_captions" sheetId="1" r:id="rId1"/>
@@ -184,9 +184,6 @@
     <t>ಶ್ರೀಮತ್ ಅಭಿನವ ರಾಮಾನುಜ ಬ್ರಹ್ಮತಂತ್ರ ಸ್ವತಂತ್ರ ಪರಕಾಲ ಮಹಾ ದೇಶಿಕನ್ (1972 – 1992)</t>
   </si>
   <si>
-    <t>ಶ್ರೀಮತ್ ಅಭಿನವ ವಾಗೀಶ ಬ್ರಹ್ಮತಂತ್ರ ಸ್ವತಂತ್ರ ಪರಕಾಲ ಮಹಾ ದೇಶಿಕನ್ (1992 – present)</t>
-  </si>
-  <si>
     <t>ಶ್ರೀ ಲಕ್ಷ್ಮಿ ಹಯಗ್ರೀವ</t>
   </si>
   <si>
@@ -257,6 +254,9 @@
   </si>
   <si>
     <t>ಶ್ರೀ ದೇವಿ</t>
+  </si>
+  <si>
+    <t>ಶ್ರೀಮತ್ ಅಭಿನವ ವಾಗೀಶ ಬ್ರಹ್ಮತಂತ್ರ ಸ್ವತಂತ್ರ ಪರಕಾಲ ಮಹಾ ದೇಶಿಕನ್ (1992 – ಪ್ರಾಕೃತ)</t>
   </si>
 </sst>
 </file>
@@ -375,7 +375,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -428,9 +428,7 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -653,7 +651,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -731,10 +729,10 @@
       <c r="A3" s="21">
         <v>2</v>
       </c>
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="25"/>
+      <c r="C3" s="24"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
@@ -1435,10 +1433,10 @@
       <c r="A25" s="21">
         <v>24</v>
       </c>
-      <c r="B25" s="26" t="s">
+      <c r="B25" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="C25" s="25"/>
+      <c r="C25" s="24"/>
       <c r="D25" s="5"/>
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
@@ -1595,10 +1593,10 @@
       <c r="A30" s="21">
         <v>29</v>
       </c>
-      <c r="B30" s="26" t="s">
+      <c r="B30" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="C30" s="25"/>
+      <c r="C30" s="24"/>
       <c r="D30" s="5"/>
       <c r="E30" s="5"/>
       <c r="F30" s="5"/>
@@ -1723,10 +1721,10 @@
       <c r="A34" s="21">
         <v>33</v>
       </c>
-      <c r="B34" s="26" t="s">
+      <c r="B34" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="C34" s="25"/>
+      <c r="C34" s="24"/>
       <c r="D34" s="5"/>
       <c r="E34" s="5"/>
       <c r="F34" s="5"/>
@@ -1755,10 +1753,10 @@
       <c r="A35" s="21">
         <v>34</v>
       </c>
-      <c r="B35" s="26" t="s">
+      <c r="B35" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="C35" s="25"/>
+      <c r="C35" s="24"/>
       <c r="D35" s="5"/>
       <c r="E35" s="5"/>
       <c r="F35" s="5"/>
@@ -1787,10 +1785,10 @@
       <c r="A36" s="21">
         <v>35</v>
       </c>
-      <c r="B36" s="26" t="s">
+      <c r="B36" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="C36" s="25"/>
+      <c r="C36" s="24"/>
       <c r="D36" s="5"/>
       <c r="E36" s="5"/>
       <c r="F36" s="5"/>
@@ -1819,10 +1817,10 @@
       <c r="A37" s="21">
         <v>36</v>
       </c>
-      <c r="B37" s="26" t="s">
-        <v>48</v>
+      <c r="B37" s="22" t="s">
+        <v>72</v>
       </c>
-      <c r="C37" s="25"/>
+      <c r="C37" s="24"/>
       <c r="D37" s="5"/>
       <c r="E37" s="5"/>
       <c r="F37" s="5"/>
@@ -28854,7 +28852,7 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D2" s="15">
         <v>0</v>
@@ -28864,8 +28862,8 @@
       <c r="A3" s="9">
         <v>1</v>
       </c>
-      <c r="C3" s="28" t="s">
-        <v>72</v>
+      <c r="C3" s="26" t="s">
+        <v>71</v>
       </c>
       <c r="D3" s="15">
         <v>1</v>
@@ -28876,7 +28874,7 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D4" s="14">
         <v>2</v>
@@ -28888,7 +28886,7 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D5" s="15">
         <v>3</v>
@@ -28900,7 +28898,7 @@
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D6" s="16">
         <v>4</v>
@@ -28912,7 +28910,7 @@
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D7" s="14">
         <v>5</v>
@@ -28924,7 +28922,7 @@
         <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D8" s="15">
         <v>6</v>
@@ -28936,7 +28934,7 @@
         <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D9" s="16">
         <v>7</v>
@@ -28948,7 +28946,7 @@
         <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D10" s="14">
         <v>8</v>
@@ -28960,7 +28958,7 @@
         <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D11" s="15">
         <v>9</v>
@@ -28974,7 +28972,7 @@
         <v>10</v>
       </c>
       <c r="C12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D12" s="15">
         <v>10</v>
@@ -28985,7 +28983,7 @@
         <v>11</v>
       </c>
       <c r="C13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D13" s="15">
         <v>10</v>
@@ -28996,7 +28994,7 @@
         <v>12</v>
       </c>
       <c r="C14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D14" s="15">
         <v>11</v>
@@ -29007,7 +29005,7 @@
         <v>13</v>
       </c>
       <c r="C15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D15" s="15">
         <v>11</v>
@@ -29018,7 +29016,7 @@
         <v>14</v>
       </c>
       <c r="C16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D16" s="15">
         <v>12</v>
@@ -29029,7 +29027,7 @@
         <v>15</v>
       </c>
       <c r="C17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D17" s="15">
         <v>12</v>
@@ -29040,7 +29038,7 @@
         <v>16</v>
       </c>
       <c r="C18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D18" s="17">
         <v>13</v>
@@ -29051,7 +29049,7 @@
         <v>17</v>
       </c>
       <c r="C19" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D19" s="17">
         <v>14</v>
@@ -29065,7 +29063,7 @@
         <v>18</v>
       </c>
       <c r="C20" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D20" s="18">
         <v>15</v>
@@ -33023,40 +33021,40 @@
       <c r="A2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="27" t="s">
-        <v>67</v>
+      <c r="B2" s="25" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="27" t="s">
-        <v>68</v>
+      <c r="B3" s="25" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="27" t="s">
-        <v>69</v>
+      <c r="B4" s="25" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="27" t="s">
-        <v>70</v>
+      <c r="B5" s="25" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="27" t="s">
-        <v>71</v>
+      <c r="B6" s="25" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Typo in Kannada spreadsheet
</commit_message>
<xml_diff>
--- a/acharyan_captions_kannada.xlsx
+++ b/acharyan_captions_kannada.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\CODING\POSTER\Sri_Parakala_Poster_Template_300DPI\Parampara_Poster\parampara_poster_template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92CA9DD5-BFA8-49A9-B6CF-A879AB1904CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DC0DC0D-BD88-460E-AB24-2AF3A8A57DEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40110" yWindow="1100" windowWidth="27580" windowHeight="19070" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="43940" yWindow="2060" windowWidth="28800" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="acharyan_captions" sheetId="1" r:id="rId1"/>
@@ -256,7 +256,7 @@
     <t>ಶ್ರೀ ದೇವಿ</t>
   </si>
   <si>
-    <t>ಶ್ರೀಮತ್ ಅಭಿನವ ವಾಗೀಶ ಬ್ರಹ್ಮತಂತ್ರ ಸ್ವತಂತ್ರ ಪರಕಾಲ ಮಹಾ ದೇಶಿಕನ್ (1992 – ಪ್ರಾಕೃತ)</t>
+    <t>ಶ್ರೀಮತ್ ಅಭಿನವ ವಾಗೀಶ ಬ್ರಹ್ಮತಂತ್ರ ಸ್ವತಂತ್ರ ಪರಕಾಲ ಮಹಾ ದೇಶಿಕನ್ (1992 – ಪ್ರಕೃತ)</t>
   </si>
 </sst>
 </file>
@@ -651,7 +651,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Some changes to Kannada
</commit_message>
<xml_diff>
--- a/acharyan_captions_kannada.xlsx
+++ b/acharyan_captions_kannada.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\CODING\POSTER\Sri_Parakala_Poster_Template_300DPI\Parampara_Poster\parampara_poster_template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8BBB783-317B-408E-80D1-BFAB83CB3648}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B84EA618-B336-45A0-954D-047EA502ED55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38460" yWindow="1280" windowWidth="28800" windowHeight="15370" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5390" yWindow="3550" windowWidth="28800" windowHeight="15370" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="acharyan_captions" sheetId="1" r:id="rId1"/>
@@ -88,22 +88,13 @@
     <t xml:space="preserve">ಸ್ವಾಮಿ ನಮ್ಮಾಳ್ವಾರ್ </t>
   </si>
   <si>
-    <t>ಶ್ರೀಮನ್ ನಾಥ ಮುನಿ</t>
-  </si>
-  <si>
     <t>ಶ್ರೀ ಉಯ್ಯಕ್ಕೊಂಡಾರ್</t>
   </si>
   <si>
     <t>ಶ್ರೀ ಮಣಕ್ಕಾಲ್ ನಂಬಿ</t>
   </si>
   <si>
-    <t>ಶ್ರೀಮದ್ ಯಾಮುನಾಚಾರ್ಯ</t>
-  </si>
-  <si>
     <t>ಶ್ರೀ ಪೆರಿಯ ನಂಬಿ</t>
-  </si>
-  <si>
-    <t>ಭಗವದ್ ರಾಮಾನುಜ</t>
   </si>
   <si>
     <t xml:space="preserve">ತಿರುಕ್ಕುರುಗೈ ಪ್ಪಿರಾನ್ ಪಿಳ್ಳಾನ್ </t>
@@ -254,6 +245,15 @@
   </si>
   <si>
     <t>ಶ್ರೀ ಬ್ರಹ್ಮತಂತ್ರ ಸ್ವತಂತ್ರ ಮಹಾದೇಶಿಕನ್ (1359 – 1386)</t>
+  </si>
+  <si>
+    <t>ಶ್ರೀಮನ್ನಾಥಮುನಿ</t>
+  </si>
+  <si>
+    <t>ಶ್ರೀಮದ್ಯಾಮುನಾಚಾರ್ಯ</t>
+  </si>
+  <si>
+    <t>ಭಗವದ್ರಾಮಾನುಜ</t>
   </si>
 </sst>
 </file>
@@ -695,7 +695,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C2" s="19"/>
       <c r="D2" s="1"/>
@@ -727,7 +727,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C3" s="24"/>
       <c r="D3" s="1"/>
@@ -759,7 +759,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C4" s="19"/>
       <c r="D4" s="1"/>
@@ -791,7 +791,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C5" s="19"/>
       <c r="D5" s="1"/>
@@ -823,7 +823,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C6" s="19"/>
       <c r="D6" s="1"/>
@@ -855,7 +855,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C7" s="19"/>
       <c r="D7" s="1"/>
@@ -887,7 +887,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C8" s="19"/>
       <c r="D8" s="1"/>
@@ -919,7 +919,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C9" s="19"/>
       <c r="D9" s="1"/>
@@ -951,7 +951,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C10" s="19"/>
       <c r="D10" s="1"/>
@@ -983,7 +983,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C11" s="19"/>
       <c r="D11" s="1"/>
@@ -1015,7 +1015,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C12" s="19"/>
       <c r="D12" s="1"/>
@@ -1047,7 +1047,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C13" s="19"/>
       <c r="D13" s="1"/>
@@ -1079,7 +1079,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C14" s="19"/>
       <c r="D14" s="1"/>
@@ -1111,7 +1111,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C15" s="19"/>
       <c r="D15" s="1"/>
@@ -1143,7 +1143,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="19" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C16" s="19"/>
       <c r="D16" s="1"/>
@@ -1175,7 +1175,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="22" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C17" s="22"/>
       <c r="D17" s="5"/>
@@ -1207,7 +1207,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="22" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C18" s="22"/>
       <c r="D18" s="5"/>
@@ -1239,7 +1239,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="22" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C19" s="22"/>
       <c r="D19" s="5"/>
@@ -1271,7 +1271,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="22" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C20" s="22"/>
       <c r="D20" s="5"/>
@@ -1303,7 +1303,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="22" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C21" s="22"/>
       <c r="D21" s="5"/>
@@ -1335,7 +1335,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="22" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C22" s="22"/>
       <c r="D22" s="5"/>
@@ -1367,7 +1367,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="22" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C23" s="22"/>
       <c r="D23" s="5"/>
@@ -1399,7 +1399,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="22" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C24" s="22"/>
       <c r="D24" s="5"/>
@@ -1431,7 +1431,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="22" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C25" s="24"/>
       <c r="D25" s="5"/>
@@ -1463,7 +1463,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="22" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C26" s="22"/>
       <c r="D26" s="5"/>
@@ -1495,7 +1495,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="22" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C27" s="22"/>
       <c r="D27" s="5"/>
@@ -1527,7 +1527,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="22" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C28" s="22"/>
       <c r="D28" s="5"/>
@@ -1559,7 +1559,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="22" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C29" s="22"/>
       <c r="D29" s="5"/>
@@ -1591,7 +1591,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="22" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C30" s="24"/>
       <c r="D30" s="5"/>
@@ -1623,7 +1623,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="22" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C31" s="22"/>
       <c r="D31" s="5"/>
@@ -1655,7 +1655,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="22" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C32" s="22"/>
       <c r="D32" s="5"/>
@@ -1687,7 +1687,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="22" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C33" s="22"/>
       <c r="D33" s="5"/>
@@ -1719,7 +1719,7 @@
         <v>33</v>
       </c>
       <c r="B34" s="22" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C34" s="24"/>
       <c r="D34" s="5"/>
@@ -1751,7 +1751,7 @@
         <v>34</v>
       </c>
       <c r="B35" s="22" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C35" s="24"/>
       <c r="D35" s="5"/>
@@ -1783,7 +1783,7 @@
         <v>35</v>
       </c>
       <c r="B36" s="22" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C36" s="24"/>
       <c r="D36" s="5"/>
@@ -1815,7 +1815,7 @@
         <v>36</v>
       </c>
       <c r="B37" s="22" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C37" s="24"/>
       <c r="D37" s="5"/>
@@ -28816,8 +28816,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0139F442-1B47-40FE-BE5B-EBE8D8F2F5C2}">
   <dimension ref="A1:E1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -28827,7 +28827,9 @@
     <col min="3" max="3" width="27.453125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.36328125" style="15" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.90625" style="13" bestFit="1" customWidth="1"/>
-    <col min="6" max="26" width="8.81640625" customWidth="1"/>
+    <col min="6" max="6" width="8.81640625" customWidth="1"/>
+    <col min="7" max="7" width="23.6328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="26" width="8.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
@@ -28860,7 +28862,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="26" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D3" s="15">
         <v>1</v>
@@ -28895,7 +28897,7 @@
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>16</v>
+        <v>69</v>
       </c>
       <c r="D6" s="16">
         <v>4</v>
@@ -28907,7 +28909,7 @@
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D7" s="14">
         <v>5</v>
@@ -28919,7 +28921,7 @@
         <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D8" s="15">
         <v>6</v>
@@ -28931,7 +28933,7 @@
         <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>19</v>
+        <v>70</v>
       </c>
       <c r="D9" s="16">
         <v>7</v>
@@ -28943,7 +28945,7 @@
         <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D10" s="14">
         <v>8</v>
@@ -28955,7 +28957,7 @@
         <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>21</v>
+        <v>71</v>
       </c>
       <c r="D11" s="15">
         <v>9</v>
@@ -28969,7 +28971,7 @@
         <v>10</v>
       </c>
       <c r="C12" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D12" s="15">
         <v>10</v>
@@ -28980,7 +28982,7 @@
         <v>11</v>
       </c>
       <c r="C13" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D13" s="15">
         <v>10</v>
@@ -28991,7 +28993,7 @@
         <v>12</v>
       </c>
       <c r="C14" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D14" s="15">
         <v>11</v>
@@ -29002,7 +29004,7 @@
         <v>13</v>
       </c>
       <c r="C15" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D15" s="15">
         <v>11</v>
@@ -29013,7 +29015,7 @@
         <v>14</v>
       </c>
       <c r="C16" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D16" s="15">
         <v>12</v>
@@ -29024,7 +29026,7 @@
         <v>15</v>
       </c>
       <c r="C17" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D17" s="15">
         <v>12</v>
@@ -29035,7 +29037,7 @@
         <v>16</v>
       </c>
       <c r="C18" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D18" s="17">
         <v>13</v>
@@ -29046,7 +29048,7 @@
         <v>17</v>
       </c>
       <c r="C19" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D19" s="17">
         <v>14</v>
@@ -29060,7 +29062,7 @@
         <v>18</v>
       </c>
       <c r="C20" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D20" s="18">
         <v>15</v>
@@ -32996,7 +32998,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8815AC1-E8BC-41ED-9BBF-007FDE576FC8}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
@@ -33019,7 +33021,7 @@
         <v>8</v>
       </c>
       <c r="B2" s="25" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -33027,7 +33029,7 @@
         <v>9</v>
       </c>
       <c r="B3" s="25" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
@@ -33035,7 +33037,7 @@
         <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
@@ -33049,7 +33051,7 @@
         <v>12</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changes in Kannada and Telugu
</commit_message>
<xml_diff>
--- a/acharyan_captions_kannada.xlsx
+++ b/acharyan_captions_kannada.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\CODING\POSTER\Sri_Parakala_Poster_Template_300DPI\Parampara_Poster\parampara_poster_template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B84EA618-B336-45A0-954D-047EA502ED55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D4D3DA22-577D-4DF9-BD8D-5E82A5D61E4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5390" yWindow="3550" windowWidth="28800" windowHeight="15370" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9010" yWindow="3800" windowWidth="28800" windowHeight="15370" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="acharyan_captions" sheetId="1" r:id="rId1"/>
@@ -125,9 +125,6 @@
   </si>
   <si>
     <t>ಶ್ರೀ ದೇವಿ</t>
-  </si>
-  <si>
-    <t>ಶ್ರೀ ವೇದಾಂತ ದೇಶಿಕರಿಂದ ಕ್ರಿ.ಶ. 1359ರ ಸಂವತ್ಸರದಲ್ಲಿ ಸ್ಥಾಪಿತವಾದುದು</t>
   </si>
   <si>
     <t>ಶ್ರೀ ಬ್ರಹ್ಮತಂತ್ರ ಸ್ವತಂತ್ರ ಪರಕಾಲ ಸ್ವಾಮಿ ಮಠದ ಆಚಾರ್ಯರು</t>
@@ -254,6 +251,9 @@
   </si>
   <si>
     <t>ಭಗವದ್ರಾಮಾನುಜ</t>
+  </si>
+  <si>
+    <t>ಶ್ರೀ ವೇದಾಂತ ದೇಶಿಕರಿಂದ 1359 ರಲ್ಲಿ ಸ್ಥಾಪಿತವಾದುದು</t>
   </si>
 </sst>
 </file>
@@ -695,7 +695,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C2" s="19"/>
       <c r="D2" s="1"/>
@@ -727,7 +727,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C3" s="24"/>
       <c r="D3" s="1"/>
@@ -759,7 +759,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C4" s="19"/>
       <c r="D4" s="1"/>
@@ -791,7 +791,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C5" s="19"/>
       <c r="D5" s="1"/>
@@ -823,7 +823,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C6" s="19"/>
       <c r="D6" s="1"/>
@@ -855,7 +855,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C7" s="19"/>
       <c r="D7" s="1"/>
@@ -887,7 +887,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C8" s="19"/>
       <c r="D8" s="1"/>
@@ -919,7 +919,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C9" s="19"/>
       <c r="D9" s="1"/>
@@ -951,7 +951,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C10" s="19"/>
       <c r="D10" s="1"/>
@@ -983,7 +983,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C11" s="19"/>
       <c r="D11" s="1"/>
@@ -1015,7 +1015,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C12" s="19"/>
       <c r="D12" s="1"/>
@@ -1047,7 +1047,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C13" s="19"/>
       <c r="D13" s="1"/>
@@ -1079,7 +1079,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C14" s="19"/>
       <c r="D14" s="1"/>
@@ -1111,7 +1111,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C15" s="19"/>
       <c r="D15" s="1"/>
@@ -1143,7 +1143,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="19" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C16" s="19"/>
       <c r="D16" s="1"/>
@@ -1175,7 +1175,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="22" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C17" s="22"/>
       <c r="D17" s="5"/>
@@ -1207,7 +1207,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="22" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C18" s="22"/>
       <c r="D18" s="5"/>
@@ -1239,7 +1239,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="22" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C19" s="22"/>
       <c r="D19" s="5"/>
@@ -1271,7 +1271,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="22" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C20" s="22"/>
       <c r="D20" s="5"/>
@@ -1303,7 +1303,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="22" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C21" s="22"/>
       <c r="D21" s="5"/>
@@ -1335,7 +1335,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="22" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C22" s="22"/>
       <c r="D22" s="5"/>
@@ -1367,7 +1367,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="22" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C23" s="22"/>
       <c r="D23" s="5"/>
@@ -1399,7 +1399,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="22" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C24" s="22"/>
       <c r="D24" s="5"/>
@@ -1431,7 +1431,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="22" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C25" s="24"/>
       <c r="D25" s="5"/>
@@ -1463,7 +1463,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="22" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C26" s="22"/>
       <c r="D26" s="5"/>
@@ -1495,7 +1495,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="22" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C27" s="22"/>
       <c r="D27" s="5"/>
@@ -1527,7 +1527,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="22" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C28" s="22"/>
       <c r="D28" s="5"/>
@@ -1559,7 +1559,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C29" s="22"/>
       <c r="D29" s="5"/>
@@ -1591,7 +1591,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="22" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C30" s="24"/>
       <c r="D30" s="5"/>
@@ -1623,7 +1623,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="22" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C31" s="22"/>
       <c r="D31" s="5"/>
@@ -1655,7 +1655,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="22" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C32" s="22"/>
       <c r="D32" s="5"/>
@@ -1687,7 +1687,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="22" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C33" s="22"/>
       <c r="D33" s="5"/>
@@ -1719,7 +1719,7 @@
         <v>33</v>
       </c>
       <c r="B34" s="22" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C34" s="24"/>
       <c r="D34" s="5"/>
@@ -1751,7 +1751,7 @@
         <v>34</v>
       </c>
       <c r="B35" s="22" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C35" s="24"/>
       <c r="D35" s="5"/>
@@ -1783,7 +1783,7 @@
         <v>35</v>
       </c>
       <c r="B36" s="22" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C36" s="24"/>
       <c r="D36" s="5"/>
@@ -1815,7 +1815,7 @@
         <v>36</v>
       </c>
       <c r="B37" s="22" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C37" s="24"/>
       <c r="D37" s="5"/>
@@ -28816,7 +28816,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0139F442-1B47-40FE-BE5B-EBE8D8F2F5C2}">
   <dimension ref="A1:E1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
@@ -28897,7 +28897,7 @@
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D6" s="16">
         <v>4</v>
@@ -28933,7 +28933,7 @@
         <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D9" s="16">
         <v>7</v>
@@ -28957,7 +28957,7 @@
         <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D11" s="15">
         <v>9</v>
@@ -29048,7 +29048,7 @@
         <v>17</v>
       </c>
       <c r="C19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D19" s="17">
         <v>14</v>
@@ -32998,8 +32998,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8815AC1-E8BC-41ED-9BBF-007FDE576FC8}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -33021,7 +33021,7 @@
         <v>8</v>
       </c>
       <c r="B2" s="25" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -33029,7 +33029,7 @@
         <v>9</v>
       </c>
       <c r="B3" s="25" t="s">
-        <v>29</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
@@ -33037,7 +33037,7 @@
         <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">

</xml_diff>